<commit_message>
Adicionado Validação por API Linguagem Natural
</commit_message>
<xml_diff>
--- a/planilhaTeste.xlsx
+++ b/planilhaTeste.xlsx
@@ -39,16 +39,16 @@
     <t>https://www.petnaturau.com/frango-comida-natural-para-caes-bh-e-regiao/</t>
   </si>
   <si>
+    <t>confere</t>
+  </si>
+  <si>
+    <t>Petisco de frango - 70g</t>
+  </si>
+  <si>
+    <t>https://www.petnaturau.com/petisco-de-frango-70g/</t>
+  </si>
+  <si>
     <t>Sem ID novo</t>
-  </si>
-  <si>
-    <t>Petisco de frango - 70g</t>
-  </si>
-  <si>
-    <t>https://www.petnaturau.com/petisco-de-frango-70g/</t>
-  </si>
-  <si>
-    <t>confere</t>
   </si>
   <si>
     <t>Filhotes - Alimentação natural - Frango (200g) (BH e região)</t>
@@ -699,7 +699,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F4" s="1" t="s"/>
       <c r="G4" s="1" t="s"/>
@@ -737,7 +737,7 @@
         <v>14</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F5" s="1" t="s"/>
       <c r="G5" s="1" t="s"/>
@@ -774,7 +774,9 @@
       <c r="D6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="1" t="s"/>
+      <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>

</xml_diff>